<commit_message>
adjust algae per day calc
</commit_message>
<xml_diff>
--- a/RAnalysis/Data/Algae_FlowCytometry/cumulative_raw/Algae_head_tank.xlsx
+++ b/RAnalysis/Data/Algae_FlowCytometry/cumulative_raw/Algae_head_tank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samjg\Documents\Github_repositories\Airradians_OA-foodsupply\RAnalysis\Data\Algae_FlowCytometry\cumulative_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{167E2B6D-B1DA-4E74-8A4F-91EB7E55D1B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3274FBA5-6279-4462-9E1A-5C934A1F0E74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4370" yWindow="1240" windowWidth="14400" windowHeight="8170" xr2:uid="{0305FFDC-29DC-4802-BD7E-06F3089E291D}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0305FFDC-29DC-4802-BD7E-06F3089E291D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -81,13 +81,37 @@
   </si>
   <si>
     <t>1,872,061 +/- 1,003,988</t>
+  </si>
+  <si>
+    <t>Num tanks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alage head tank fed to 8 tanks </t>
+  </si>
+  <si>
+    <t>Peristaltic was 2 mL per minute</t>
+  </si>
+  <si>
+    <t>Flow rate (mL per minute)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Flow rate per day </t>
+  </si>
+  <si>
+    <t>mL algae per high-food tank per day!</t>
+  </si>
+  <si>
+    <t>High chl cells per day per tank ==[ (mean high chl cells as cells mL * mL per tank per day) / 8]</t>
+  </si>
+  <si>
+    <t>Low chl cells per day per tank ==[ (mean high chl cells as cells mL * mL per tank per day) / 8]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -100,6 +124,14 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,11 +154,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097D929C-BACD-45F2-AABF-85837FEA58AC}">
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D4" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" topLeftCell="D22" workbookViewId="0">
+      <selection activeCell="J27" sqref="J27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1075,6 +1108,71 @@
         <v>1003987.5723013718</v>
       </c>
     </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G28" t="s">
+        <v>16</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I29">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G30" t="s">
+        <v>17</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="I31">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="G32" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="7:12" x14ac:dyDescent="0.35">
+      <c r="H33" s="4">
+        <f>I31*60*24</f>
+        <v>2880</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="4"/>
+    </row>
+    <row r="35" spans="7:12" x14ac:dyDescent="0.35">
+      <c r="G35" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="7:12" x14ac:dyDescent="0.35">
+      <c r="G36">
+        <f>(H22*H33)/8</f>
+        <v>341210311.00478464</v>
+      </c>
+    </row>
+    <row r="37" spans="7:12" x14ac:dyDescent="0.35">
+      <c r="G37" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="38" spans="7:12" x14ac:dyDescent="0.35">
+      <c r="G38">
+        <f>(H25*H33)/8</f>
+        <v>673942105.26315784</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>